<commit_message>
Efficiency update motor and motor controller
</commit_message>
<xml_diff>
--- a/Documents/sense_analysis_IOM.xlsx
+++ b/Documents/sense_analysis_IOM.xlsx
@@ -10,12 +10,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="32">
   <si>
     <t>Sensitivity Testing IOM</t>
   </si>
@@ -35,9 +35,6 @@
     <t>delta energy</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
     <t>name and initial</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>efficiency</t>
+  </si>
+  <si>
+    <t>wind_speed</t>
   </si>
   <si>
     <t>rider_mass</t>
@@ -117,12 +117,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="GENERAL" numFmtId="165"/>
   </numFmts>
   <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -143,6 +145,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
@@ -190,17 +193,21 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
@@ -220,25 +227,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="F1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F14" activeCellId="0" pane="topLeft" sqref="F14"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C108" activeCellId="0" pane="topLeft" sqref="C108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.9336734693878"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.6683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6581632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.7142857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5714285714286"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -248,7 +255,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="2">
       <c r="G2" s="0" t="s">
         <v>2</v>
       </c>
@@ -261,75 +268,72 @@
       <c r="J2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="n">
         <f aca="false">D5</f>
         <v>0</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="3" t="n">
         <f aca="false">D6</f>
         <v>-24.6000000000058</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="3" t="n">
         <f aca="false">D7</f>
         <v>850.199999999997</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="3" t="n">
         <f aca="false">D8</f>
         <v>-0.299999999999272</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="n">
         <f aca="false">$C$3*(1+0.15)</f>
         <v>0.115</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="3" t="n">
         <f aca="false">$C$3*(1-0.15)</f>
         <v>0.085</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="n">
         <f aca="false">D12</f>
         <v>-1.90000000000001</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="3" t="n">
         <f aca="false">D13</f>
         <v>-3389.7</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="3" t="n">
         <f aca="false">D14</f>
         <v>-18862.3</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="3" t="n">
         <f aca="false">D15</f>
         <v>-829.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>116</v>
@@ -337,33 +341,33 @@
       <c r="C5" s="0" t="n">
         <v>116</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="3" t="n">
         <f aca="false">B5 - C5</f>
         <v>0</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="n">
         <f aca="false">D19</f>
         <v>2.91</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="3" t="n">
         <f aca="false">D20</f>
         <v>5362.1</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="3" t="n">
         <f aca="false">D21</f>
         <v>21665.8</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="3" t="n">
         <f aca="false">D22</f>
         <v>1317.9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>53419.2</v>
@@ -371,33 +375,33 @@
       <c r="C6" s="0" t="n">
         <v>53443.8</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="3" t="n">
         <f aca="false">B6 - C6</f>
         <v>-24.6000000000058</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="n">
         <f aca="false">D26</f>
         <v>0</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="3" t="n">
         <f aca="false">D27</f>
         <v>-79.4000000000015</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="3" t="n">
         <f aca="false">D28</f>
         <v>885.800000000003</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="3" t="n">
         <f aca="false">D29</f>
         <v>-13.7000000000007</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>105286.2</v>
@@ -405,33 +409,33 @@
       <c r="C7" s="0" t="n">
         <v>104436</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="3" t="n">
         <f aca="false">B7 - C7</f>
         <v>850.199999999997</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="n">
         <f aca="false">D33</f>
         <v>0.5</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="3" t="n">
         <f aca="false">D34</f>
         <v>136.099999999999</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="3" t="n">
         <f aca="false">D35</f>
         <v>24.5999999999913</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="3" t="n">
         <f aca="false">D36</f>
         <v>-22.7000000000007</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>17212.5</v>
@@ -439,120 +443,120 @@
       <c r="C8" s="0" t="n">
         <v>17212.8</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="3" t="n">
         <f aca="false">B8 - C8</f>
         <v>-0.299999999999272</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3" t="n">
         <f aca="false">D40</f>
         <v>-0.5</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="3" t="n">
         <f aca="false">D41</f>
         <v>-394.700000000004</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="3" t="n">
         <f aca="false">D42</f>
         <v>1146.8</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="3" t="n">
         <f aca="false">D43</f>
         <v>-59.2000000000007</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
-      <c r="D9" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="9">
+      <c r="D9" s="3" t="n">
         <f aca="false">B9 - C9</f>
         <v>0</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="n">
         <f aca="false">D47</f>
         <v>-3.3</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="3" t="n">
         <f aca="false">D48</f>
         <v>-42130.5</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="3" t="n">
         <f aca="false">D49</f>
         <v>-7626.7</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="3" t="n">
         <f aca="false">D50</f>
         <v>3410.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0.323596</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G10" s="3" t="n">
         <f aca="false">D54</f>
         <v>-3.3</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="3" t="n">
         <f aca="false">D55</f>
         <v>-42130.5</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="3" t="n">
         <f aca="false">D56</f>
         <v>-7626.7</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="3" t="n">
         <f aca="false">D57</f>
         <v>3410.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="n">
         <f aca="false">$C$10*(1+0.15)</f>
         <v>0.3721354</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="3" t="n">
         <f aca="false">$C$10*(1-0.15)</f>
         <v>0.2750566</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G11" s="3" t="n">
         <f aca="false">D61</f>
         <v>-3.3</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="3" t="n">
         <f aca="false">D62</f>
         <v>-42130.5</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="3" t="n">
         <f aca="false">D63</f>
         <v>-7626.7</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="3" t="n">
         <f aca="false">D64</f>
         <v>3410.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>113.8</v>
@@ -560,33 +564,33 @@
       <c r="C12" s="0" t="n">
         <v>115.7</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="3" t="n">
         <f aca="false">B12 - C12</f>
         <v>-1.90000000000001</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3" t="n">
         <f aca="false">D68</f>
         <v>0</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="3" t="n">
         <f aca="false">D69</f>
         <v>0</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="3" t="n">
         <f aca="false">D70</f>
         <v>0</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12" s="3" t="n">
         <f aca="false">D71</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>49302.5</v>
@@ -594,33 +598,33 @@
       <c r="C13" s="0" t="n">
         <v>52692.2</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="3" t="n">
         <f aca="false">B13 - C13</f>
         <v>-3389.7</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G13" s="3" t="n">
         <f aca="false">D75</f>
         <v>4.2</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="3" t="n">
         <f aca="false">D76</f>
         <v>507684.4</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="3" t="n">
         <f aca="false">D77</f>
         <v>36932.4</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J13" s="3" t="n">
         <f aca="false">D78</f>
         <v>1878.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>91306.2</v>
@@ -628,33 +632,33 @@
       <c r="C14" s="0" t="n">
         <v>110168.5</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="3" t="n">
         <f aca="false">B14 - C14</f>
         <v>-18862.3</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G14" s="3" t="n">
         <f aca="false">D82</f>
         <v>2.7</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="3" t="n">
         <f aca="false">D83</f>
         <v>2359.6</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="3" t="n">
         <f aca="false">D84</f>
         <v>11586.9</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="J14" s="3" t="n">
         <f aca="false">D85</f>
         <v>360.700000000001</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>16191.1</v>
@@ -662,63 +666,82 @@
       <c r="C15" s="0" t="n">
         <v>17020.7</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="3" t="n">
         <f aca="false">B15 - C15</f>
         <v>-829.6</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G15" s="3" t="n">
         <f aca="false">D89</f>
         <v>0</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="3" t="n">
         <f aca="false">D90</f>
         <v>-16331</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="3" t="n">
         <f aca="false">D91</f>
         <v>-32310.2</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="3" t="n">
         <f aca="false">D92</f>
         <v>-18783</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="16">
-      <c r="D16" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="16">
+      <c r="D16" s="3" t="n">
         <f aca="false">B16 - C16</f>
         <v>0</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="17">
+      <c r="F16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <f aca="false">D96</f>
+        <v>-1.5</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <f aca="false">D97</f>
+        <v>254</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <f aca="false">D98</f>
+        <v>-2310.90000000001</v>
+      </c>
+      <c r="J16" s="3" t="n">
+        <f aca="false">D99</f>
+        <v>323.700000000001</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>2.174</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3" t="n">
         <f aca="false">$C$17*(1+0.15)</f>
         <v>2.5001</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="3" t="n">
         <f aca="false">$C$17*(1-0.15)</f>
         <v>1.8479</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>116.3</v>
@@ -726,14 +749,14 @@
       <c r="C19" s="0" t="n">
         <v>113.39</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="3" t="n">
         <f aca="false">B19 - C19</f>
         <v>2.91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>53895.2</v>
@@ -741,14 +764,14 @@
       <c r="C20" s="0" t="n">
         <v>48533.1</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="3" t="n">
         <f aca="false">B20 - C20</f>
         <v>5362.1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>110192.5</v>
@@ -756,14 +779,14 @@
       <c r="C21" s="0" t="n">
         <v>88526.7</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="3" t="n">
         <f aca="false">B21 - C21</f>
         <v>21665.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>17319.6</v>
@@ -771,20 +794,20 @@
       <c r="C22" s="0" t="n">
         <v>16001.7</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="3" t="n">
         <f aca="false">B22 - C22</f>
         <v>1317.9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="23">
-      <c r="D23" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="23">
+      <c r="D23" s="3" t="n">
         <f aca="false">B23 - C23</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>28</v>
@@ -793,22 +816,22 @@
         <v>81.64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B25" s="3" t="n">
         <f aca="false">$C$24*(1+0.15)</f>
         <v>93.886</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="3" t="n">
         <f aca="false">$C$24*(1-0.15)</f>
         <v>69.394</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>116</v>
@@ -816,14 +839,14 @@
       <c r="C26" s="0" t="n">
         <v>116</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="3" t="n">
         <f aca="false">B26 - C26</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>53388.6</v>
@@ -831,14 +854,14 @@
       <c r="C27" s="0" t="n">
         <v>53468</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="3" t="n">
         <f aca="false">B27 - C27</f>
         <v>-79.4000000000015</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>105128.7</v>
@@ -846,14 +869,14 @@
       <c r="C28" s="0" t="n">
         <v>104242.9</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="3" t="n">
         <f aca="false">B28 - C28</f>
         <v>885.800000000003</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>17204.1</v>
@@ -861,20 +884,20 @@
       <c r="C29" s="0" t="n">
         <v>17217.8</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="3" t="n">
         <f aca="false">B29 - C29</f>
         <v>-13.7000000000007</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="30">
-      <c r="D30" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="30">
+      <c r="D30" s="3" t="n">
         <f aca="false">B30 - C30</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>29</v>
@@ -883,22 +906,22 @@
         <v>226.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B32" s="3" t="n">
         <f aca="false">$C$31*(1+0.15)</f>
         <v>260.705</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C32" s="3" t="n">
         <f aca="false">$C$31*(1-0.15)</f>
         <v>192.695</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>116</v>
@@ -906,14 +929,14 @@
       <c r="C33" s="0" t="n">
         <v>115.5</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="3" t="n">
         <f aca="false">B33 - C33</f>
         <v>0.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>53348</v>
@@ -921,14 +944,14 @@
       <c r="C34" s="0" t="n">
         <v>53211.9</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="3" t="n">
         <f aca="false">B34 - C34</f>
         <v>136.099999999999</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>105301.9</v>
@@ -936,14 +959,14 @@
       <c r="C35" s="0" t="n">
         <v>105277.3</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="3" t="n">
         <f aca="false">B35 - C35</f>
         <v>24.5999999999913</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>17191</v>
@@ -951,44 +974,44 @@
       <c r="C36" s="0" t="n">
         <v>17213.7</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="3" t="n">
         <f aca="false">B36 - C36</f>
         <v>-22.7000000000007</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="37">
-      <c r="D37" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="37">
+      <c r="D37" s="3" t="n">
         <f aca="false">B37 - C37</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>9.81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B39" s="3" t="n">
         <f aca="false">$C$38*(1+0.15)</f>
         <v>11.2815</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="3" t="n">
         <f aca="false">$C$38*(1-0.15)</f>
         <v>8.3385</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>115.6</v>
@@ -996,14 +1019,14 @@
       <c r="C40" s="0" t="n">
         <v>116.1</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D40" s="3" t="n">
         <f aca="false">B40 - C40</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>53144.2</v>
@@ -1011,14 +1034,14 @@
       <c r="C41" s="0" t="n">
         <v>53538.9</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41" s="3" t="n">
         <f aca="false">B41 - C41</f>
         <v>-394.700000000004</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>105729.2</v>
@@ -1026,14 +1049,14 @@
       <c r="C42" s="0" t="n">
         <v>104582.4</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="3" t="n">
         <f aca="false">B42 - C42</f>
         <v>1146.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>17175.5</v>
@@ -1041,44 +1064,44 @@
       <c r="C43" s="0" t="n">
         <v>17234.7</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="3" t="n">
         <f aca="false">B43 - C43</f>
         <v>-59.2000000000007</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="44">
-      <c r="D44" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="44">
+      <c r="D44" s="3" t="n">
         <f aca="false">B44 - C44</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>0.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B46" s="3" t="n">
         <f aca="false">$C$45*(1+0.15)</f>
         <v>0.805</v>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="C46" s="3" t="n">
         <f aca="false">$C$45*(1-0.15)</f>
         <v>0.595</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="47">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>113.9</v>
@@ -1086,14 +1109,14 @@
       <c r="C47" s="0" t="n">
         <v>117.2</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="D47" s="3" t="n">
         <f aca="false">B47 - C47</f>
         <v>-3.3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>5672.3</v>
@@ -1101,14 +1124,14 @@
       <c r="C48" s="0" t="n">
         <v>47802.8</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="D48" s="3" t="n">
         <f aca="false">B48 - C48</f>
         <v>-42130.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="49">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>101604</v>
@@ -1116,14 +1139,14 @@
       <c r="C49" s="0" t="n">
         <v>109230.7</v>
       </c>
-      <c r="D49" s="0" t="n">
+      <c r="D49" s="3" t="n">
         <f aca="false">B49 - C49</f>
         <v>-7626.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="50">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>18653.3</v>
@@ -1131,44 +1154,44 @@
       <c r="C50" s="0" t="n">
         <v>15242.6</v>
       </c>
-      <c r="D50" s="0" t="n">
+      <c r="D50" s="3" t="n">
         <f aca="false">B50 - C50</f>
         <v>3410.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="51">
-      <c r="D51" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="51">
+      <c r="D51" s="3" t="n">
         <f aca="false">B51 - C51</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>1.204</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="53">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B53" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B53" s="3" t="n">
         <f aca="false">$C$45*(1+0.15)</f>
         <v>0.805</v>
       </c>
-      <c r="C53" s="0" t="n">
+      <c r="C53" s="3" t="n">
         <f aca="false">$C$45*(1-0.15)</f>
         <v>0.595</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="54">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>113.9</v>
@@ -1176,14 +1199,14 @@
       <c r="C54" s="0" t="n">
         <v>117.2</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="D54" s="3" t="n">
         <f aca="false">B54 - C54</f>
         <v>-3.3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="55">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>5672.3</v>
@@ -1191,14 +1214,14 @@
       <c r="C55" s="0" t="n">
         <v>47802.8</v>
       </c>
-      <c r="D55" s="0" t="n">
+      <c r="D55" s="3" t="n">
         <f aca="false">B55 - C55</f>
         <v>-42130.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>101604</v>
@@ -1206,14 +1229,14 @@
       <c r="C56" s="0" t="n">
         <v>109230.7</v>
       </c>
-      <c r="D56" s="0" t="n">
+      <c r="D56" s="3" t="n">
         <f aca="false">B56 - C56</f>
         <v>-7626.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="57">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>18653.3</v>
@@ -1221,20 +1244,20 @@
       <c r="C57" s="0" t="n">
         <v>15242.6</v>
       </c>
-      <c r="D57" s="0" t="n">
+      <c r="D57" s="3" t="n">
         <f aca="false">B57 - C57</f>
         <v>3410.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="58">
-      <c r="D58" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="58">
+      <c r="D58" s="3" t="n">
         <f aca="false">B58 - C58</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="59">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>30</v>
@@ -1243,22 +1266,22 @@
         <v>0.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="60">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B60" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B60" s="3" t="n">
         <f aca="false">$C$45*(1+0.15)</f>
         <v>0.805</v>
       </c>
-      <c r="C60" s="0" t="n">
+      <c r="C60" s="3" t="n">
         <f aca="false">$C$45*(1-0.15)</f>
         <v>0.595</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>113.9</v>
@@ -1266,14 +1289,14 @@
       <c r="C61" s="0" t="n">
         <v>117.2</v>
       </c>
-      <c r="D61" s="0" t="n">
+      <c r="D61" s="3" t="n">
         <f aca="false">B61 - C61</f>
         <v>-3.3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="62">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>5672.3</v>
@@ -1281,14 +1304,14 @@
       <c r="C62" s="0" t="n">
         <v>47802.8</v>
       </c>
-      <c r="D62" s="0" t="n">
+      <c r="D62" s="3" t="n">
         <f aca="false">B62 - C62</f>
         <v>-42130.5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="63">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>101604</v>
@@ -1296,14 +1319,14 @@
       <c r="C63" s="0" t="n">
         <v>109230.7</v>
       </c>
-      <c r="D63" s="0" t="n">
+      <c r="D63" s="3" t="n">
         <f aca="false">B63 - C63</f>
         <v>-7626.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="64">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>18653.3</v>
@@ -1311,44 +1334,44 @@
       <c r="C64" s="0" t="n">
         <v>15242.6</v>
       </c>
-      <c r="D64" s="0" t="n">
+      <c r="D64" s="3" t="n">
         <f aca="false">B64 - C64</f>
         <v>3410.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="65">
-      <c r="D65" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="65">
+      <c r="D65" s="3" t="n">
         <f aca="false">B65 - C65</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>0.022</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="67">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B67" s="3" t="n">
         <f aca="false">$C$66*(1+0.15)</f>
         <v>0.0253</v>
       </c>
-      <c r="C67" s="0" t="n">
+      <c r="C67" s="3" t="n">
         <f aca="false">$C$66*(1-0.15)</f>
         <v>0.0187</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="68">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>116</v>
@@ -1356,14 +1379,14 @@
       <c r="C68" s="0" t="n">
         <v>116</v>
       </c>
-      <c r="D68" s="0" t="n">
+      <c r="D68" s="3" t="n">
         <f aca="false">B68 - C68</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>53416.3</v>
@@ -1371,14 +1394,14 @@
       <c r="C69" s="0" t="n">
         <v>53416.3</v>
       </c>
-      <c r="D69" s="0" t="n">
+      <c r="D69" s="3" t="n">
         <f aca="false">B69 - C69</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="70">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>105257.2</v>
@@ -1386,14 +1409,14 @@
       <c r="C70" s="0" t="n">
         <v>105257.2</v>
       </c>
-      <c r="D70" s="0" t="n">
+      <c r="D70" s="3" t="n">
         <f aca="false">B70 - C70</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="71">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>17210</v>
@@ -1401,20 +1424,20 @@
       <c r="C71" s="0" t="n">
         <v>17210</v>
       </c>
-      <c r="D71" s="0" t="n">
+      <c r="D71" s="3" t="n">
         <f aca="false">B71 - C71</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="72">
-      <c r="D72" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="72">
+      <c r="D72" s="3" t="n">
         <f aca="false">B72 - C72</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="73">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>31</v>
@@ -1423,22 +1446,22 @@
         <v>200</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B74" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B74" s="3" t="n">
         <f aca="false">$C$73*(1+0.15)</f>
         <v>230</v>
       </c>
-      <c r="C74" s="0" t="n">
+      <c r="C74" s="3" t="n">
         <f aca="false">$C$73*(1-0.15)</f>
         <v>170</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="75">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>117.3</v>
@@ -1446,14 +1469,14 @@
       <c r="C75" s="0" t="n">
         <v>113.1</v>
       </c>
-      <c r="D75" s="0" t="n">
+      <c r="D75" s="3" t="n">
         <f aca="false">B75 - C75</f>
         <v>4.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>556142.4</v>
@@ -1461,14 +1484,14 @@
       <c r="C76" s="0" t="n">
         <v>48458</v>
       </c>
-      <c r="D76" s="0" t="n">
+      <c r="D76" s="3" t="n">
         <f aca="false">B76 - C76</f>
         <v>507684.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="77">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>124052.3</v>
@@ -1476,14 +1499,14 @@
       <c r="C77" s="0" t="n">
         <v>87119.9</v>
       </c>
-      <c r="D77" s="0" t="n">
+      <c r="D77" s="3" t="n">
         <f aca="false">B77 - C77</f>
         <v>36932.4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="78">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>17890.8</v>
@@ -1491,44 +1514,44 @@
       <c r="C78" s="0" t="n">
         <v>16012</v>
       </c>
-      <c r="D78" s="0" t="n">
+      <c r="D78" s="3" t="n">
         <f aca="false">B78 - C78</f>
         <v>1878.8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="79">
-      <c r="D79" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="79">
+      <c r="D79" s="3" t="n">
         <f aca="false">B79 - C79</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>5000</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="81">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B81" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B81" s="3" t="n">
         <f aca="false">$C$80*(1+0.15)</f>
         <v>5750</v>
       </c>
-      <c r="C81" s="0" t="n">
+      <c r="C81" s="3" t="n">
         <f aca="false">$C$80*(1-0.15)</f>
         <v>4250</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>115.5</v>
@@ -1536,14 +1559,14 @@
       <c r="C82" s="0" t="n">
         <v>112.8</v>
       </c>
-      <c r="D82" s="0" t="n">
+      <c r="D82" s="3" t="n">
         <f aca="false">B82 - C82</f>
         <v>2.7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>53211.9</v>
@@ -1551,14 +1574,14 @@
       <c r="C83" s="0" t="n">
         <v>50852.3</v>
       </c>
-      <c r="D83" s="0" t="n">
+      <c r="D83" s="3" t="n">
         <f aca="false">B83 - C83</f>
         <v>2359.6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="84">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>105277.3</v>
@@ -1566,14 +1589,14 @@
       <c r="C84" s="0" t="n">
         <v>93690.4</v>
       </c>
-      <c r="D84" s="0" t="n">
+      <c r="D84" s="3" t="n">
         <f aca="false">B84 - C84</f>
         <v>11586.9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="85">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>17213.7</v>
@@ -1581,44 +1604,44 @@
       <c r="C85" s="0" t="n">
         <v>16853</v>
       </c>
-      <c r="D85" s="0" t="n">
+      <c r="D85" s="3" t="n">
         <f aca="false">B85 - C85</f>
         <v>360.700000000001</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="86">
-      <c r="D86" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="86">
+      <c r="D86" s="3" t="n">
         <f aca="false">B86 - C86</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="87">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>0.95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="88">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B88" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B88" s="3" t="n">
         <f aca="false">$C$87*(1+0.15)</f>
         <v>1.0925</v>
       </c>
-      <c r="C88" s="0" t="n">
+      <c r="C88" s="3" t="n">
         <f aca="false">$C$87*(1-0.15)</f>
         <v>0.8075</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="89">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>115.5</v>
@@ -1626,14 +1649,14 @@
       <c r="C89" s="0" t="n">
         <v>115.5</v>
       </c>
-      <c r="D89" s="0" t="n">
+      <c r="D89" s="3" t="n">
         <f aca="false">B89 - C89</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="90">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>46271.2</v>
@@ -1641,14 +1664,14 @@
       <c r="C90" s="0" t="n">
         <v>62602.2</v>
       </c>
-      <c r="D90" s="0" t="n">
+      <c r="D90" s="3" t="n">
         <f aca="false">B90 - C90</f>
         <v>-16331</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="91">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="91">
       <c r="A91" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>91545.5</v>
@@ -1656,14 +1679,14 @@
       <c r="C91" s="0" t="n">
         <v>123855.7</v>
       </c>
-      <c r="D91" s="0" t="n">
+      <c r="D91" s="3" t="n">
         <f aca="false">B91 - C91</f>
         <v>-32310.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="92">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="92">
       <c r="A92" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>1468.4</v>
@@ -1671,14 +1694,101 @@
       <c r="C92" s="0" t="n">
         <v>20251.4</v>
       </c>
-      <c r="D92" s="0" t="n">
+      <c r="D92" s="3" t="n">
         <f aca="false">B92 - C92</f>
         <v>-18783</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="93">
-      <c r="D93" s="0" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="93">
+      <c r="D93" s="3" t="n">
         <f aca="false">B93 - C93</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="94">
+      <c r="A94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="95">
+      <c r="A95" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" s="0" t="n">
+        <v>14.95</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>11.05</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="96">
+      <c r="A96" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96" s="0" t="n">
+        <v>105.2</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>106.7</v>
+      </c>
+      <c r="D96" s="3" t="n">
+        <f aca="false">B96-C96</f>
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="97">
+      <c r="A97" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>56406.7</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>56152.7</v>
+      </c>
+      <c r="D97" s="3" t="n">
+        <f aca="false">B97-C97</f>
+        <v>254</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="98">
+      <c r="A98" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>87717.9</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>90028.8</v>
+      </c>
+      <c r="D98" s="3" t="n">
+        <f aca="false">B98-C98</f>
+        <v>-2310.90000000001</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="99">
+      <c r="A99" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>20062.2</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>19738.5</v>
+      </c>
+      <c r="D99" s="3" t="n">
+        <f aca="false">B99-C99</f>
+        <v>323.700000000001</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="100">
+      <c r="D100" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>